<commit_message>
scraping data into excel file, fully done
</commit_message>
<xml_diff>
--- a/scraped_data.xlsx
+++ b/scraped_data.xlsx
@@ -4,16 +4,25 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet sheetId="1" name="My Sheet" state="visible" r:id="rId4"/>
+    <sheet sheetId="1" name="Sheet 1" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
   <si>
-    <t>Hello, World!</t>
+    <t>{"name":"Dreams &amp; Nightmares Case","price":"$1.33 USD"}</t>
+  </si>
+  <si>
+    <t>{"name":"Dreams &amp; Nightmares Case","price":"$1.36 USD"}</t>
+  </si>
+  <si>
+    <t>{"name":"Dreams &amp; Nightmares Case","price":"$1.37 USD"}</t>
+  </si>
+  <si>
+    <t>{"name":"Dreams &amp; Nightmares Case","price":"$1.38 USD"}</t>
   </si>
 </sst>
 </file>
@@ -390,12 +399,37 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C3:C3"/>
+  <dimension ref="A2:A7"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
-    <row r="3" spans="3:3" x14ac:dyDescent="0.25">
-      <c r="C3" t="s">
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
         <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
five items in a loop
</commit_message>
<xml_diff>
--- a/scraped_data.xlsx
+++ b/scraped_data.xlsx
@@ -11,18 +11,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="4">
-  <si>
-    <t>{"name":"Dreams &amp; Nightmares Case","price":"$1.33 USD"}</t>
-  </si>
-  <si>
-    <t>{"name":"Dreams &amp; Nightmares Case","price":"$1.36 USD"}</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
   <si>
     <t>{"name":"Dreams &amp; Nightmares Case","price":"$1.37 USD"}</t>
   </si>
   <si>
-    <t>{"name":"Dreams &amp; Nightmares Case","price":"$1.38 USD"}</t>
+    <t>{"name":"Revolution Case","price":"$1.43 USD"}</t>
+  </si>
+  <si>
+    <t>{"name":"Fracture Case","price":"$0.66 USD"}</t>
+  </si>
+  <si>
+    <t>{"name":"Paris 2023 Legends Sticker Capsule","price":"$0.26 USD"}</t>
+  </si>
+  <si>
+    <t>{"name":"Mann Co. Supply Crate Key","price":"$2.15 USD"}</t>
   </si>
 </sst>
 </file>
@@ -399,37 +402,32 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:A7"/>
+  <dimension ref="A1:A5"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+    </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1</v>
+        <v>2</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="6" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>3</v>
+        <v>4</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
testing commands for excel
</commit_message>
<xml_diff>
--- a/scraped_data.xlsx
+++ b/scraped_data.xlsx
@@ -19,13 +19,13 @@
     <t>{"name":"Revolution Case","price":"$1.43 USD"}</t>
   </si>
   <si>
-    <t>{"name":"Fracture Case","price":"$0.66 USD"}</t>
+    <t>{"name":"Paris 2023 Contenders Sticker Capsule","price":"$0.25 USD"}</t>
   </si>
   <si>
-    <t>{"name":"Paris 2023 Legends Sticker Capsule","price":"$0.26 USD"}</t>
+    <t>{"name":"Fracture Case","price":"$0.63 USD"}</t>
   </si>
   <si>
-    <t>{"name":"Mann Co. Supply Crate Key","price":"$2.15 USD"}</t>
+    <t>{"name":"Recoil Case","price":"$0.63 USD"}</t>
   </si>
 </sst>
 </file>

</xml_diff>

<commit_message>
trying to scrape items from my inventory
</commit_message>
<xml_diff>
--- a/scraped_data.xlsx
+++ b/scraped_data.xlsx
@@ -11,21 +11,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="1">
   <si>
-    <t>{"name":"Dreams &amp; Nightmares Case","price":"$1.37 USD"}</t>
-  </si>
-  <si>
-    <t>{"name":"Revolution Case","price":"$1.43 USD"}</t>
-  </si>
-  <si>
-    <t>{"name":"Paris 2023 Contenders Sticker Capsule","price":"$0.25 USD"}</t>
-  </si>
-  <si>
-    <t>{"name":"Fracture Case","price":"$0.63 USD"}</t>
-  </si>
-  <si>
-    <t>{"name":"Recoil Case","price":"$0.63 USD"}</t>
+    <t>Paris 2023 Challengers Sticker Capsule</t>
   </si>
 </sst>
 </file>
@@ -402,7 +390,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A5"/>
+  <dimension ref="A1:A4"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="1" spans="1:1" x14ac:dyDescent="0.25">
@@ -412,22 +400,17 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
     </row>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>4</v>
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
final for today, some troubles with links
</commit_message>
<xml_diff>
--- a/scraped_data.xlsx
+++ b/scraped_data.xlsx
@@ -11,9 +11,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="1">
   <si>
-    <t>Paris 2023 Challengers Sticker Capsule</t>
+    <t>Paris 2023 Contenders Sticker Capsule</t>
   </si>
 </sst>
 </file>
@@ -403,16 +403,8 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>0</v>
-      </c>
-    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
scrping info from four pages, but it takes to long
</commit_message>
<xml_diff>
--- a/scraped_data.xlsx
+++ b/scraped_data.xlsx
@@ -11,9 +11,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="1">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
   <si>
     <t>Paris 2023 Contenders Sticker Capsule</t>
+  </si>
+  <si>
+    <t>Paris 2023 Legends Sticker Capsule</t>
+  </si>
+  <si>
+    <t>Paris 2023 Challengers Sticker Capsule</t>
+  </si>
+  <si>
+    <t>Dreams &amp; Nightmares Case</t>
   </si>
 </sst>
 </file>
@@ -400,11 +409,19 @@
     </row>
     <row r="2" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>0</v>
+        <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
've tryed some ways to fix an error, but nothing helps
</commit_message>
<xml_diff>
--- a/scraped_data.xlsx
+++ b/scraped_data.xlsx
@@ -11,18 +11,12 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
   <si>
     <t>Paris 2023 Contenders Sticker Capsule</t>
   </si>
   <si>
     <t>Paris 2023 Legends Sticker Capsule</t>
-  </si>
-  <si>
-    <t>Paris 2023 Challengers Sticker Capsule</t>
-  </si>
-  <si>
-    <t>Dreams &amp; Nightmares Case</t>
   </si>
 </sst>
 </file>
@@ -412,16 +406,8 @@
         <v>1</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
works even with bug, not sure if im able to fix it
</commit_message>
<xml_diff>
--- a/scraped_data.xlsx
+++ b/scraped_data.xlsx
@@ -4,21 +4,10 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet sheetId="1" name="Sheet 1" state="visible" r:id="rId4"/>
+    <sheet sheetId="1" name="Sheet 1" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t>Paris 2023 Contenders Sticker Capsule</t>
-  </si>
-  <si>
-    <t>Paris 2023 Legends Sticker Capsule</t>
-  </si>
-</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -396,16 +385,8 @@
   <dimension ref="A1:A4"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-    </row>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25"/>
     <row r="3" spans="1:1" x14ac:dyDescent="0.25"/>
     <row r="4" spans="1:1" x14ac:dyDescent="0.25"/>
   </sheetData>

</xml_diff>

<commit_message>
proper sending of data to teble's cells
</commit_message>
<xml_diff>
--- a/scraped_data.xlsx
+++ b/scraped_data.xlsx
@@ -4,10 +4,21 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet sheetId="1" name="Sheet 1" state="visible" r:id="rId3"/>
+    <sheet sheetId="1" name="Sheet 1" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+  <si>
+    <t>Paris 2023 Contenders Sticker Capsule</t>
+  </si>
+  <si>
+    <t>$0.28 USD</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -382,13 +393,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:B1"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.25"/>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
first attempt to scratch 4 sites
</commit_message>
<xml_diff>
--- a/scraped_data.xlsx
+++ b/scraped_data.xlsx
@@ -4,21 +4,10 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet sheetId="1" name="Sheet 1" state="visible" r:id="rId4"/>
+    <sheet sheetId="1" name="Sheet 1" state="visible" r:id="rId3"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
-</file>
-
-<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
-  <si>
-    <t>Paris 2023 Contenders Sticker Capsule</t>
-  </si>
-  <si>
-    <t>$0.28 USD</t>
-  </si>
-</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -393,17 +382,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B1"/>
+  <dimension ref="A2:B5"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25"/>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25"/>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
afters some fixes it works
</commit_message>
<xml_diff>
--- a/scraped_data.xlsx
+++ b/scraped_data.xlsx
@@ -4,10 +4,36 @@
   <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="164011" filterPrivacy="1"/>
   <sheets>
-    <sheet sheetId="1" name="Sheet 1" state="visible" r:id="rId3"/>
+    <sheet sheetId="1" name="Sheet 1" state="visible" r:id="rId4"/>
   </sheets>
   <calcPr calcId="171027"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="7">
+  <si>
+    <t>Paris 2023 Contenders Sticker Capsule</t>
+  </si>
+  <si>
+    <t>$0.28 USD</t>
+  </si>
+  <si>
+    <t>Paris 2023 Legends Sticker Capsule</t>
+  </si>
+  <si>
+    <t>Paris 2023 Challengers Sticker Capsule</t>
+  </si>
+  <si>
+    <t>Dreams &amp; Nightmares Case</t>
+  </si>
+  <si>
+    <t>$1.28 USD</t>
+  </si>
+  <si>
+    <t>$1.27 USD</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -382,13 +408,98 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:B5"/>
+  <dimension ref="A2:B13"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25"/>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25"/>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>3</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25"/>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>2</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A8" t="s">
+        <v>3</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A9" t="s">
+        <v>4</v>
+      </c>
+      <c r="B9" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>2</v>
+      </c>
+      <c r="B11" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>3</v>
+      </c>
+      <c r="B12" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>4</v>
+      </c>
+      <c r="B13" t="s">
+        <v>5</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="4294967295" verticalDpi="4294967295" scale="100" fitToWidth="1" fitToHeight="1"/>

</xml_diff>

<commit_message>
good sending data to excel table
</commit_message>
<xml_diff>
--- a/scraped_data.xlsx
+++ b/scraped_data.xlsx
@@ -11,7 +11,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="7">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
   <si>
     <t>Paris 2023 Contenders Sticker Capsule</t>
   </si>
@@ -28,10 +28,7 @@
     <t>Dreams &amp; Nightmares Case</t>
   </si>
   <si>
-    <t>$1.28 USD</t>
-  </si>
-  <si>
-    <t>$1.27 USD</t>
+    <t>$1.26 USD</t>
   </si>
 </sst>
 </file>
@@ -408,7 +405,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:B13"/>
+  <dimension ref="A2:B5"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
     <row r="2" spans="1:2" x14ac:dyDescent="0.25">
@@ -440,63 +437,6 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25"/>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>2</v>
-      </c>
-      <c r="B7" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A8" t="s">
-        <v>3</v>
-      </c>
-      <c r="B8" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>4</v>
-      </c>
-      <c r="B9" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>2</v>
-      </c>
-      <c r="B11" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A12" t="s">
-        <v>3</v>
-      </c>
-      <c r="B12" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A13" t="s">
-        <v>4</v>
-      </c>
-      <c r="B13" t="s">
         <v>5</v>
       </c>
     </row>

</xml_diff>

<commit_message>
some design and code changes
</commit_message>
<xml_diff>
--- a/scraped_data.xlsx
+++ b/scraped_data.xlsx
@@ -11,7 +11,13 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="8">
+  <si>
+    <t>Items</t>
+  </si>
+  <si>
+    <t>Prices</t>
+  </si>
   <si>
     <t>Paris 2023 Contenders Sticker Capsule</t>
   </si>
@@ -28,7 +34,7 @@
     <t>Dreams &amp; Nightmares Case</t>
   </si>
   <si>
-    <t>$1.28 USD</t>
+    <t>$1.24 USD</t>
   </si>
 </sst>
 </file>
@@ -44,12 +50,17 @@
       <name val="Calibri"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF0000"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -64,8 +75,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -405,39 +417,51 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A2:B5"/>
+  <dimension ref="A1:C5"/>
   <sheetFormatPr defaultRowHeight="15" outlineLevelRow="0" outlineLevelCol="0" x14ac:dyDescent="55"/>
   <sheetData>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="1" spans="2:3" x14ac:dyDescent="0.25">
+      <c r="B1" t="s">
         <v>0</v>
       </c>
+      <c r="C1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A2" s="1"/>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>2</v>
+      </c>
+      <c r="C2" t="s">
+        <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A3" s="1"/>
       <c r="B3" t="s">
-        <v>1</v>
+        <v>4</v>
+      </c>
+      <c r="C3" t="s">
+        <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A4" s="1"/>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+      <c r="C4" t="s">
         <v>3</v>
       </c>
-      <c r="B4" t="s">
-        <v>1</v>
-      </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A5" s="1"/>
       <c r="B5" t="s">
-        <v>5</v>
+        <v>6</v>
+      </c>
+      <c r="C5" t="s">
+        <v>7</v>
       </c>
     </row>
   </sheetData>

</xml_diff>